<commit_message>
Update test and grades
</commit_message>
<xml_diff>
--- a/Documentation/ADP Project Rubrics.xlsx
+++ b/Documentation/ADP Project Rubrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_UserData\GitHub\Repos\adp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364BE2B6-8739-421D-8F6C-E56F9A89A1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF112EE-D985-4208-980E-93E3A4DC82BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADP B_Impl" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="63">
   <si>
     <t>Acceptatiecriteria</t>
   </si>
@@ -680,8 +680,8 @@
   <dimension ref="A1:Y1058"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2449,7 +2449,9 @@
       <c r="E51" s="21">
         <v>0</v>
       </c>
-      <c r="F51" s="21"/>
+      <c r="F51" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
@@ -2486,7 +2488,9 @@
       <c r="E52" s="20">
         <v>0</v>
       </c>
-      <c r="F52" s="20"/>
+      <c r="F52" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
@@ -2523,7 +2527,9 @@
       <c r="E53" s="20">
         <v>1</v>
       </c>
-      <c r="F53" s="20"/>
+      <c r="F53" s="20">
+        <v>1</v>
+      </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
@@ -2620,7 +2626,9 @@
       <c r="E56" s="21">
         <v>2</v>
       </c>
-      <c r="F56" s="21"/>
+      <c r="F56" s="21">
+        <v>2</v>
+      </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2719,7 +2727,9 @@
       <c r="E59" s="21">
         <v>4</v>
       </c>
-      <c r="F59" s="21"/>
+      <c r="F59" s="21">
+        <v>4</v>
+      </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2820,7 +2830,9 @@
       <c r="E62" s="21">
         <v>4</v>
       </c>
-      <c r="F62" s="21"/>
+      <c r="F62" s="21">
+        <v>4</v>
+      </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -2853,7 +2865,7 @@
       </c>
       <c r="F63" s="26">
         <f>SUM(F53:F62)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G63" s="17"/>
       <c r="H63" s="17"/>
@@ -2922,7 +2934,9 @@
       <c r="E65" s="21">
         <v>0</v>
       </c>
-      <c r="F65" s="21"/>
+      <c r="F65" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
@@ -2959,7 +2973,9 @@
       <c r="E66" s="20">
         <v>0</v>
       </c>
-      <c r="F66" s="20"/>
+      <c r="F66" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G66" s="14"/>
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
@@ -2996,7 +3012,9 @@
       <c r="E67" s="20">
         <v>1</v>
       </c>
-      <c r="F67" s="20"/>
+      <c r="F67" s="20">
+        <v>1</v>
+      </c>
       <c r="G67" s="14"/>
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
@@ -3093,7 +3111,9 @@
       <c r="E70" s="21">
         <v>2</v>
       </c>
-      <c r="F70" s="21"/>
+      <c r="F70" s="21">
+        <v>2</v>
+      </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -3192,7 +3212,9 @@
       <c r="E73" s="21">
         <v>4</v>
       </c>
-      <c r="F73" s="21"/>
+      <c r="F73" s="21">
+        <v>4</v>
+      </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -3293,7 +3315,9 @@
       <c r="E76" s="21">
         <v>4</v>
       </c>
-      <c r="F76" s="21"/>
+      <c r="F76" s="21">
+        <v>4</v>
+      </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
@@ -3326,7 +3350,7 @@
       </c>
       <c r="F77" s="26">
         <f>SUM(F67:F76)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G77" s="17"/>
       <c r="H77" s="17"/>
@@ -3395,7 +3419,9 @@
       <c r="E79" s="21">
         <v>0</v>
       </c>
-      <c r="F79" s="21"/>
+      <c r="F79" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
@@ -3432,7 +3458,9 @@
       <c r="E80" s="20">
         <v>0</v>
       </c>
-      <c r="F80" s="20"/>
+      <c r="F80" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
@@ -3469,7 +3497,9 @@
       <c r="E81" s="20">
         <v>1</v>
       </c>
-      <c r="F81" s="20"/>
+      <c r="F81" s="20">
+        <v>1</v>
+      </c>
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
@@ -3566,7 +3596,9 @@
       <c r="E84" s="21">
         <v>2</v>
       </c>
-      <c r="F84" s="21"/>
+      <c r="F84" s="21">
+        <v>2</v>
+      </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
@@ -3665,7 +3697,9 @@
       <c r="E87" s="21">
         <v>4</v>
       </c>
-      <c r="F87" s="21"/>
+      <c r="F87" s="21">
+        <v>4</v>
+      </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -3766,7 +3800,9 @@
       <c r="E90" s="21">
         <v>4</v>
       </c>
-      <c r="F90" s="21"/>
+      <c r="F90" s="21">
+        <v>4</v>
+      </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
@@ -3799,7 +3835,7 @@
       </c>
       <c r="F91" s="26">
         <f>SUM(F81:F90)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G91" s="17"/>
       <c r="H91" s="17"/>
@@ -7672,7 +7708,7 @@
       </c>
       <c r="F206" s="27">
         <f>1+((F203+F189+F175+F161+F147+F133+F119+F105+F91+F77+F63+F49+F35+F21+F7)/(E203+E189+E175+E161+E147+E133+E119+E105+E91+E77+E63+E49+E35+E21+E7))*9</f>
-        <v>2.6875</v>
+        <v>4.5437499999999993</v>
       </c>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>

</xml_diff>

<commit_message>
Implement Graph and Dijkstra algoritme and add unittests for Graph
</commit_message>
<xml_diff>
--- a/Documentation/ADP Project Rubrics.xlsx
+++ b/Documentation/ADP Project Rubrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_UserData\GitHub\Repos\adp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF112EE-D985-4208-980E-93E3A4DC82BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AE2537-81BE-4726-83F3-D01318E9861A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="63">
   <si>
     <t>Acceptatiecriteria</t>
   </si>
@@ -680,8 +680,8 @@
   <dimension ref="A1:Y1058"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3904,7 +3904,9 @@
       <c r="E93" s="21">
         <v>0</v>
       </c>
-      <c r="F93" s="21"/>
+      <c r="F93" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
@@ -3941,7 +3943,9 @@
       <c r="E94" s="20">
         <v>0</v>
       </c>
-      <c r="F94" s="20"/>
+      <c r="F94" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
@@ -3978,7 +3982,9 @@
       <c r="E95" s="20">
         <v>1</v>
       </c>
-      <c r="F95" s="20"/>
+      <c r="F95" s="20">
+        <v>1</v>
+      </c>
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
@@ -4075,7 +4081,9 @@
       <c r="E98" s="21">
         <v>2</v>
       </c>
-      <c r="F98" s="21"/>
+      <c r="F98" s="21">
+        <v>2</v>
+      </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
@@ -4174,7 +4182,9 @@
       <c r="E101" s="21">
         <v>4</v>
       </c>
-      <c r="F101" s="21"/>
+      <c r="F101" s="21">
+        <v>4</v>
+      </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
@@ -4275,7 +4285,9 @@
       <c r="E104" s="21">
         <v>4</v>
       </c>
-      <c r="F104" s="21"/>
+      <c r="F104" s="21">
+        <v>4</v>
+      </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
@@ -4308,7 +4320,7 @@
       </c>
       <c r="F105" s="26">
         <f>SUM(F95:F104)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G105" s="17"/>
       <c r="H105" s="17"/>
@@ -4377,7 +4389,9 @@
       <c r="E107" s="21">
         <v>0</v>
       </c>
-      <c r="F107" s="21"/>
+      <c r="F107" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
@@ -4414,7 +4428,9 @@
       <c r="E108" s="20">
         <v>0</v>
       </c>
-      <c r="F108" s="20"/>
+      <c r="F108" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G108" s="14"/>
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
@@ -4451,7 +4467,9 @@
       <c r="E109" s="20">
         <v>1</v>
       </c>
-      <c r="F109" s="20"/>
+      <c r="F109" s="20">
+        <v>1</v>
+      </c>
       <c r="G109" s="14"/>
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
@@ -4548,7 +4566,9 @@
       <c r="E112" s="21">
         <v>2</v>
       </c>
-      <c r="F112" s="21"/>
+      <c r="F112" s="21">
+        <v>2</v>
+      </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
@@ -4647,7 +4667,9 @@
       <c r="E115" s="21">
         <v>4</v>
       </c>
-      <c r="F115" s="21"/>
+      <c r="F115" s="21">
+        <v>4</v>
+      </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -4748,7 +4770,9 @@
       <c r="E118" s="21">
         <v>4</v>
       </c>
-      <c r="F118" s="21"/>
+      <c r="F118" s="21">
+        <v>4</v>
+      </c>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -4781,7 +4805,7 @@
       </c>
       <c r="F119" s="26">
         <f>SUM(F109:F118)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G119" s="17"/>
       <c r="H119" s="17"/>
@@ -4850,7 +4874,9 @@
       <c r="E121" s="21">
         <v>0</v>
       </c>
-      <c r="F121" s="21"/>
+      <c r="F121" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -4887,7 +4913,9 @@
       <c r="E122" s="20">
         <v>0</v>
       </c>
-      <c r="F122" s="20"/>
+      <c r="F122" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G122" s="14"/>
       <c r="H122" s="14"/>
       <c r="I122" s="14"/>
@@ -4924,7 +4952,9 @@
       <c r="E123" s="20">
         <v>1</v>
       </c>
-      <c r="F123" s="20"/>
+      <c r="F123" s="20">
+        <v>1</v>
+      </c>
       <c r="G123" s="14"/>
       <c r="H123" s="14"/>
       <c r="I123" s="14"/>
@@ -5021,7 +5051,9 @@
       <c r="E126" s="21">
         <v>2</v>
       </c>
-      <c r="F126" s="21"/>
+      <c r="F126" s="21">
+        <v>2</v>
+      </c>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -5120,7 +5152,9 @@
       <c r="E129" s="21">
         <v>4</v>
       </c>
-      <c r="F129" s="21"/>
+      <c r="F129" s="21">
+        <v>4</v>
+      </c>
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
@@ -5221,7 +5255,9 @@
       <c r="E132" s="21">
         <v>4</v>
       </c>
-      <c r="F132" s="21"/>
+      <c r="F132" s="21">
+        <v>4</v>
+      </c>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
@@ -5254,7 +5290,7 @@
       </c>
       <c r="F133" s="26">
         <f>SUM(F123:F132)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G133" s="17"/>
       <c r="H133" s="17"/>
@@ -5323,7 +5359,9 @@
       <c r="E135" s="21">
         <v>0</v>
       </c>
-      <c r="F135" s="21"/>
+      <c r="F135" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
@@ -5360,7 +5398,9 @@
       <c r="E136" s="20">
         <v>0</v>
       </c>
-      <c r="F136" s="20"/>
+      <c r="F136" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
@@ -5397,7 +5437,9 @@
       <c r="E137" s="20">
         <v>1</v>
       </c>
-      <c r="F137" s="20"/>
+      <c r="F137" s="20">
+        <v>1</v>
+      </c>
       <c r="G137" s="14"/>
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
@@ -5494,7 +5536,9 @@
       <c r="E140" s="21">
         <v>2</v>
       </c>
-      <c r="F140" s="21"/>
+      <c r="F140" s="21">
+        <v>2</v>
+      </c>
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -5593,7 +5637,9 @@
       <c r="E143" s="21">
         <v>4</v>
       </c>
-      <c r="F143" s="21"/>
+      <c r="F143" s="21">
+        <v>4</v>
+      </c>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -5694,7 +5740,9 @@
       <c r="E146" s="21">
         <v>4</v>
       </c>
-      <c r="F146" s="21"/>
+      <c r="F146" s="21">
+        <v>4</v>
+      </c>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -5727,7 +5775,7 @@
       </c>
       <c r="F147" s="26">
         <f>SUM(F137:F146)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G147" s="17"/>
       <c r="H147" s="17"/>
@@ -7708,7 +7756,7 @@
       </c>
       <c r="F206" s="27">
         <f>1+((F203+F189+F175+F161+F147+F133+F119+F105+F91+F77+F63+F49+F35+F21+F7)/(E203+E189+E175+E161+E147+E133+E119+E105+E91+E77+E63+E49+E35+E21+E7))*9</f>
-        <v>4.5437499999999993</v>
+        <v>7.0187499999999998</v>
       </c>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>

</xml_diff>